<commit_message>
accountName test script updated
</commit_message>
<xml_diff>
--- a/data/customer-names.xlsx
+++ b/data/customer-names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasanthvb/Documents/CRS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasanthvb/Documents/Automation/Playwright/playwright-api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C979A8A-BA58-224C-852E-BB10E78FDBC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5F2454-65DF-9B49-A832-11F1D7CE4EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="900" windowWidth="28040" windowHeight="17180" xr2:uid="{324146B1-D5DC-8C48-9BC0-91C34FCD58E0}"/>
   </bookViews>
@@ -36,21 +36,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Business</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>CVS PHARMACY</t>
+  </si>
+  <si>
+    <t>CVS/PHARMACY</t>
+  </si>
+  <si>
+    <t>WAL-MART</t>
+  </si>
+  <si>
+    <t>WALMART</t>
+  </si>
+  <si>
+    <t>actualName</t>
+  </si>
+  <si>
+    <t>expectedName</t>
   </si>
 </sst>
 </file>
@@ -425,30 +428,30 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>

</xml_diff>